<commit_message>
Progress on generation of Veins and VeinsPreset elements
</commit_message>
<xml_diff>
--- a/Sprocket2 Spreadsheet.xlsx
+++ b/Sprocket2 Spreadsheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gits\Sprocket\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gits\COG_Config_Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="277">
   <si>
     <t>minecraft:clay</t>
   </si>
@@ -1157,6 +1157,30 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>Lots of iron</t>
+  </si>
+  <si>
+    <t>LotsOfIron</t>
+  </si>
+  <si>
+    <t>minecraft:stone, 0.75; minecraft:iron_ore, 0.25;</t>
+  </si>
+  <si>
+    <t>.*,1.00;</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>filename</t>
+  </si>
+  <si>
+    <t>0_presets.xml</t>
+  </si>
+  <si>
+    <t>1_vanilla.xml</t>
   </si>
 </sst>
 </file>
@@ -1438,7 +1462,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyBorder="1">
@@ -1498,6 +1522,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1530,7 +1557,286 @@
     <cellStyle name="Input - Fixed Width" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="64">
+  <dxfs count="113">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1555,6 +1861,45 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -1597,9 +1942,6 @@
         <vertAlign val="baseline"/>
         <sz val="8"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
@@ -1654,174 +1996,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1863,7 +2037,7 @@
   <autoFilter ref="A9:D20"/>
   <tableColumns count="4">
     <tableColumn id="1" name="ID Before" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="4" name="x" dataDxfId="63" dataCellStyle="Normal">
+    <tableColumn id="4" name="x" dataDxfId="112" dataCellStyle="Normal">
       <calculatedColumnFormula>"… will be replaced by ..."</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" name="ID After" dataCellStyle="Input - Fixed Width"/>
@@ -1874,127 +2048,128 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="StandardGen_Presets" displayName="StandardGen_Presets" ref="A8:AE12" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59" dataCellStyle="Input - Fixed Width">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="StandardGen_Presets" displayName="StandardGen_Presets" ref="A8:AE12" totalsRowShown="0" headerRowDxfId="111" dataDxfId="110" dataCellStyle="Input - Fixed Width">
   <tableColumns count="31">
-    <tableColumn id="1" name="Type" dataDxfId="58" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="61" name="OFF?" dataDxfId="57" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="74" name="Description" dataDxfId="56" dataCellStyle="Input"/>
-    <tableColumn id="2" name="name" dataDxfId="55" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="3" name="seed" dataDxfId="54" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="4" name="inherits" dataDxfId="53" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="58" name="Child of other distribution" dataDxfId="52" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="5" name="color" dataDxfId="51" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="27" name="OreBlock" dataDxfId="50" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="44" name="Replaces" dataDxfId="49" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="43" name="ReplacesOre" dataDxfId="48" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="42" name="ReplacesRegExp" dataDxfId="47" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="41" name="PlacesAbove (not implemented in Sprocket2)" dataDxfId="46" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="40" name="PlacesBelow (not implemented in Sprocket2)" dataDxfId="45" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="39" name="PlacesBeside (not implemented in Sprocket2)" dataDxfId="44" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="48" name="Biome" dataDxfId="43" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="49" name="BiomeType" dataDxfId="42" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="50" name="BiomeSet" dataDxfId="41" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="73" name="Dimension" dataDxfId="40" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="6" name="Size_avg" dataDxfId="39" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="7" name="Size_range" dataDxfId="38" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="8" name="Size_type" dataDxfId="37" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="9" name="Frequency_avg" dataDxfId="36" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="10" name="Frequency_range" dataDxfId="35" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="11" name="Frequency_type" dataDxfId="34" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="12" name="Height_avg" dataDxfId="33" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="13" name="Height_range" dataDxfId="32" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="14" name="Height_type" dataDxfId="31" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="15" name="ParentRangeLimit_avg" dataDxfId="30" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="16" name="ParentRangeLimit_range" dataDxfId="29" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="17" name="ParentRangeLimit_type" dataDxfId="28" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="1" name="Type" dataDxfId="109" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="61" name="OFF?" dataDxfId="108" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="74" name="Description" dataDxfId="107" dataCellStyle="Input"/>
+    <tableColumn id="2" name="name" dataDxfId="106" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="3" name="seed" dataDxfId="105" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="4" name="inherits" dataDxfId="104" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="58" name="Child of other distribution" dataDxfId="103" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="5" name="color" dataDxfId="102" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="27" name="OreBlock" dataDxfId="101" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="44" name="Replaces" dataDxfId="100" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="43" name="ReplacesOre" dataDxfId="99" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="42" name="ReplacesRegExp" dataDxfId="98" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="41" name="PlacesAbove (not implemented in Sprocket2)" dataDxfId="97" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="40" name="PlacesBelow (not implemented in Sprocket2)" dataDxfId="96" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="39" name="PlacesBeside (not implemented in Sprocket2)" dataDxfId="95" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="48" name="Biome" dataDxfId="94" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="49" name="BiomeType" dataDxfId="93" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="50" name="BiomeSet" dataDxfId="92" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="73" name="Dimension" dataDxfId="91" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="6" name="Size_avg" dataDxfId="90" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="7" name="Size_range" dataDxfId="89" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="8" name="Size_type" dataDxfId="88" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="9" name="Frequency_avg" dataDxfId="87" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="10" name="Frequency_range" dataDxfId="86" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="11" name="Frequency_type" dataDxfId="85" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="12" name="Height_avg" dataDxfId="84" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="13" name="Height_range" dataDxfId="83" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="14" name="Height_type" dataDxfId="82" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="15" name="ParentRangeLimit_avg" dataDxfId="81" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="16" name="ParentRangeLimit_range" dataDxfId="80" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="17" name="ParentRangeLimit_type" dataDxfId="79" dataCellStyle="Input - Fixed Width"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Veins_Presets" displayName="Veins_Presets" ref="A8:BP18" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" dataCellStyle="Input - Fixed Width">
-  <tableColumns count="68">
-    <tableColumn id="1" name="Type" dataDxfId="23" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="61" name="OFF?" dataDxfId="22" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="74" name="Description" dataDxfId="21" dataCellStyle="Input"/>
-    <tableColumn id="2" name="name" dataDxfId="20" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="3" name="seed" dataDxfId="19" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="4" name="inherits" dataDxfId="18" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="58" name="Child of other distribution" dataDxfId="17" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="5" name="color" dataDxfId="16" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="109" name="branchType" dataDxfId="15" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="27" name="OreBlock" dataDxfId="14" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="44" name="Replaces" dataDxfId="13" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="43" name="ReplacesOre" dataDxfId="12" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="42" name="ReplacesRegExp" dataDxfId="11" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="41" name="PlacesAbove (not implemented in Sprocket2)" dataDxfId="10" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="40" name="PlacesBelow (not implemented in Sprocket2)" dataDxfId="9" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="39" name="PlacesBeside (not implemented in Sprocket2)" dataDxfId="8" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="48" name="Biome" dataDxfId="7" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="49" name="BiomeType" dataDxfId="6" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="50" name="BiomeSet (not implemented in Sprocket2)" dataDxfId="5" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="73" name="Dimension" dataDxfId="4" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="6" name="OreDensity_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="7" name="OreDensity_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="8" name="OreDensity_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="9" name="OreRadiusMult_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="10" name="OreRadiusMult_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="11" name="OreRadiusMult_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="12" name="MotherlodeFrequency_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="13" name="MotherlodeFrequency_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="14" name="MotherlodeFrequency_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="15" name="MotherlodeRangeLimit_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="16" name="MotherlodeRangeLimit_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="17" name="MotherlodeRangeLimit_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="75" name="MotherlodeSize_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="76" name="MotherlodeSize_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="77" name="MotherlodeSize_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="78" name="MotherlodeHeight_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="79" name="MotherlodeHeight_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="80" name="MotherlodeHeight_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="81" name="BranchFrequency_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="82" name="BranchFrequency_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="83" name="BranchFrequency_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="84" name="BranchInclination_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="85" name="BranchInclination_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="86" name="BranchInclination_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="87" name="BranchLength_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="88" name="BranchLength_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="89" name="BranchLength_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="90" name="BranchHeightLimit_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="91" name="BranchHeightLimit_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="92" name="BranchHeightLimit_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="93" name="SegmentForkFrequency_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="94" name="SegmentForkFrequency_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="95" name="SegmentForkFrequency_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="96" name="SegmentForkLengthMult_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="97" name="SegmentForkLengthMult_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="98" name="SegmentForkLengthMult_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="99" name="SegmentLength_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="100" name="SegmentLength_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="101" name="SegmentLength_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="102" name="SegmentAngle_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="103" name="SegmentAngle_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="104" name="SegmentAngle_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="112" name="SegmentPitch_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="111" name="SegmentPitch_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="110" name="SegmentPitch_type" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="105" name="SegmentRadius_avg" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="106" name="SegmentRadius_range" dataCellStyle="Input - Fixed Width"/>
-    <tableColumn id="107" name="SegmentRadius_type" dataCellStyle="Input - Fixed Width"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Veins_Presets" displayName="Veins_Presets" ref="A8:BQ18" totalsRowShown="0" headerRowDxfId="78" dataDxfId="5" dataCellStyle="Input - Fixed Width">
+  <tableColumns count="69">
+    <tableColumn id="1" name="Type" dataDxfId="73" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="61" name="OFF?" dataDxfId="72" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="74" name="Description" dataDxfId="71" dataCellStyle="Input"/>
+    <tableColumn id="2" name="name" dataDxfId="70" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="18" name="filename" dataDxfId="0" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="3" name="seed" dataDxfId="69" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="4" name="inherits" dataDxfId="68" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="58" name="Child of other distribution" dataDxfId="67" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="5" name="color" dataDxfId="66" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="109" name="branchType" dataDxfId="65" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="27" name="OreBlock" dataDxfId="64" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="44" name="Replaces" dataDxfId="63" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="43" name="ReplacesOre" dataDxfId="62" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="42" name="ReplacesRegExp" dataDxfId="61" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="41" name="PlacesAbove (not implemented in Sprocket2)" dataDxfId="60" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="40" name="PlacesBelow (not implemented in Sprocket2)" dataDxfId="59" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="39" name="PlacesBeside (not implemented in Sprocket2)" dataDxfId="58" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="48" name="Biome" dataDxfId="57" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="49" name="BiomeType" dataDxfId="56" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="50" name="BiomeSet (not implemented in Sprocket2)" dataDxfId="55" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="73" name="Dimension" dataDxfId="54" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="6" name="OreDensity_avg" dataDxfId="53" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="7" name="OreDensity_range" dataDxfId="52" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="8" name="OreDensity_type" dataDxfId="51" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="9" name="OreRadiusMult_avg" dataDxfId="50" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="10" name="OreRadiusMult_range" dataDxfId="49" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="11" name="OreRadiusMult_type" dataDxfId="48" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="12" name="MotherlodeFrequency_avg" dataDxfId="47" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="13" name="MotherlodeFrequency_range" dataDxfId="46" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="14" name="MotherlodeFrequency_type" dataDxfId="45" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="15" name="MotherlodeRangeLimit_avg" dataDxfId="44" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="16" name="MotherlodeRangeLimit_range" dataDxfId="43" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="17" name="MotherlodeRangeLimit_type" dataDxfId="42" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="75" name="MotherlodeSize_avg" dataDxfId="41" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="76" name="MotherlodeSize_range" dataDxfId="40" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="77" name="MotherlodeSize_type" dataDxfId="39" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="78" name="MotherlodeHeight_avg" dataDxfId="38" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="79" name="MotherlodeHeight_range" dataDxfId="37" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="80" name="MotherlodeHeight_type" dataDxfId="36" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="81" name="BranchFrequency_avg" dataDxfId="35" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="82" name="BranchFrequency_range" dataDxfId="34" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="83" name="BranchFrequency_type" dataDxfId="33" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="84" name="BranchInclination_avg" dataDxfId="32" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="85" name="BranchInclination_range" dataDxfId="31" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="86" name="BranchInclination_type" dataDxfId="30" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="87" name="BranchLength_avg" dataDxfId="29" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="88" name="BranchLength_range" dataDxfId="28" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="89" name="BranchLength_type" dataDxfId="27" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="90" name="BranchHeightLimit_avg" dataDxfId="26" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="91" name="BranchHeightLimit_range" dataDxfId="25" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="92" name="BranchHeightLimit_type" dataDxfId="24" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="93" name="SegmentForkFrequency_avg" dataDxfId="23" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="94" name="SegmentForkFrequency_range" dataDxfId="22" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="95" name="SegmentForkFrequency_type" dataDxfId="21" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="96" name="SegmentForkLengthMult_avg" dataDxfId="20" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="97" name="SegmentForkLengthMult_range" dataDxfId="19" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="98" name="SegmentForkLengthMult_type" dataDxfId="18" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="99" name="SegmentLength_avg" dataDxfId="17" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="100" name="SegmentLength_range" dataDxfId="16" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="101" name="SegmentLength_type" dataDxfId="15" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="102" name="SegmentAngle_avg" dataDxfId="14" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="103" name="SegmentAngle_range" dataDxfId="13" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="104" name="SegmentAngle_type" dataDxfId="12" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="112" name="SegmentPitch_avg" dataDxfId="11" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="111" name="SegmentPitch_range" dataDxfId="10" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="110" name="SegmentPitch_type" dataDxfId="9" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="105" name="SegmentRadius_avg" dataDxfId="8" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="106" name="SegmentRadius_range" dataDxfId="7" dataCellStyle="Input - Fixed Width"/>
+    <tableColumn id="107" name="SegmentRadius_type" dataDxfId="6" dataCellStyle="Input - Fixed Width"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A3:C24" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A3:C24" totalsRowShown="0" dataDxfId="77">
   <autoFilter ref="A3:C24"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Column Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Typical Value" dataDxfId="1"/>
-    <tableColumn id="3" name="Explanation" dataDxfId="0"/>
+    <tableColumn id="1" name="Column Name" dataDxfId="76"/>
+    <tableColumn id="2" name="Typical Value" dataDxfId="75"/>
+    <tableColumn id="3" name="Explanation" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2518,12 +2693,12 @@
     </row>
     <row r="6" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:31" ht="30" x14ac:dyDescent="0.4">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="13"/>
@@ -2531,36 +2706,36 @@
       <c r="I7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="31" t="s">
+      <c r="J7" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="27" t="s">
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
+      <c r="Q7" s="28"/>
+      <c r="R7" s="28"/>
       <c r="S7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="T7" s="28" t="s">
+      <c r="T7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="U7" s="29"/>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
-      <c r="AD7" s="29"/>
-      <c r="AE7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="31"/>
     </row>
     <row r="8" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
@@ -2889,12 +3064,12 @@
     <mergeCell ref="J7:O7"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:AE12">
-    <cfRule type="notContainsBlanks" dxfId="62" priority="6">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="containsText" dxfId="61" priority="1" operator="containsText" text="OFF">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="OFF">
       <formula>NOT(ISERROR(SEARCH("OFF",B9)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2908,13 +3083,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP18"/>
+  <dimension ref="A1:BQ18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="8" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="8" topLeftCell="E14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2923,140 +3098,142 @@
     <col min="2" max="2" width="5.625" customWidth="1"/>
     <col min="3" max="3" width="30.625" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
-    <col min="6" max="7" width="25.625" customWidth="1"/>
-    <col min="8" max="9" width="15.625" customWidth="1"/>
-    <col min="10" max="13" width="40.625" customWidth="1"/>
-    <col min="14" max="16" width="10.625" style="9" customWidth="1"/>
-    <col min="17" max="18" width="25.625" customWidth="1"/>
-    <col min="19" max="19" width="10.625" customWidth="1"/>
-    <col min="20" max="20" width="25.625" customWidth="1"/>
-    <col min="21" max="68" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="8" width="25.625" customWidth="1"/>
+    <col min="9" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="14" width="40.625" customWidth="1"/>
+    <col min="15" max="17" width="10.625" style="9" customWidth="1"/>
+    <col min="18" max="19" width="25.625" customWidth="1"/>
+    <col min="20" max="20" width="10.625" customWidth="1"/>
+    <col min="21" max="21" width="25.625" customWidth="1"/>
+    <col min="22" max="69" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:69" ht="30" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>267</v>
       </c>
-      <c r="M2" s="9"/>
-      <c r="P2"/>
-    </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="N2" s="9"/>
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>265</v>
       </c>
-      <c r="M3" s="9"/>
-      <c r="P3"/>
-    </row>
-    <row r="4" spans="1:68" ht="15" x14ac:dyDescent="0.25">
+      <c r="N3" s="9"/>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:69" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>268</v>
       </c>
-      <c r="M4" s="9"/>
-      <c r="P4"/>
-    </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.2">
+      <c r="N4" s="9"/>
+      <c r="Q4"/>
+    </row>
+    <row r="5" spans="1:69" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>266</v>
       </c>
-      <c r="M5" s="9"/>
-      <c r="P5"/>
-    </row>
-    <row r="6" spans="1:68" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:68" ht="30" x14ac:dyDescent="0.4">
-      <c r="A7" s="25" t="s">
+      <c r="N5" s="9"/>
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:69" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:69" ht="30" x14ac:dyDescent="0.4">
+      <c r="A7" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="12"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="25"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="15" t="s">
+      <c r="G7" s="12"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="L7" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="27" t="s">
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="18" t="s">
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="U7" s="28" t="s">
+      <c r="V7" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="V7" s="29"/>
-      <c r="W7" s="29"/>
-      <c r="X7" s="29"/>
-      <c r="Y7" s="29"/>
-      <c r="Z7" s="29"/>
-      <c r="AA7" s="29"/>
-      <c r="AB7" s="29"/>
-      <c r="AC7" s="29"/>
-      <c r="AD7" s="29"/>
-      <c r="AE7" s="29"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="30"/>
+      <c r="AE7" s="30"/>
       <c r="AF7" s="30"/>
-      <c r="AG7" s="28" t="s">
+      <c r="AG7" s="31"/>
+      <c r="AH7" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="AH7" s="29"/>
-      <c r="AI7" s="29"/>
-      <c r="AJ7" s="29"/>
-      <c r="AK7" s="29"/>
-      <c r="AL7" s="29"/>
-      <c r="AM7" s="29"/>
-      <c r="AN7" s="29"/>
-      <c r="AO7" s="29"/>
-      <c r="AP7" s="29"/>
-      <c r="AQ7" s="29"/>
+      <c r="AI7" s="30"/>
+      <c r="AJ7" s="30"/>
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="30"/>
+      <c r="AM7" s="30"/>
+      <c r="AN7" s="30"/>
+      <c r="AO7" s="30"/>
+      <c r="AP7" s="30"/>
+      <c r="AQ7" s="30"/>
       <c r="AR7" s="30"/>
-      <c r="AS7" s="28" t="s">
+      <c r="AS7" s="31"/>
+      <c r="AT7" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="AT7" s="29"/>
-      <c r="AU7" s="29"/>
-      <c r="AV7" s="29"/>
-      <c r="AW7" s="29"/>
-      <c r="AX7" s="29"/>
-      <c r="AY7" s="29"/>
-      <c r="AZ7" s="29"/>
-      <c r="BA7" s="29"/>
-      <c r="BB7" s="29"/>
-      <c r="BC7" s="29"/>
+      <c r="AU7" s="30"/>
+      <c r="AV7" s="30"/>
+      <c r="AW7" s="30"/>
+      <c r="AX7" s="30"/>
+      <c r="AY7" s="30"/>
+      <c r="AZ7" s="30"/>
+      <c r="BA7" s="30"/>
+      <c r="BB7" s="30"/>
+      <c r="BC7" s="30"/>
       <c r="BD7" s="30"/>
-      <c r="BE7" s="28" t="s">
+      <c r="BE7" s="31"/>
+      <c r="BF7" s="29" t="s">
         <v>135</v>
       </c>
-      <c r="BF7" s="29"/>
-      <c r="BG7" s="29"/>
-      <c r="BH7" s="29"/>
-      <c r="BI7" s="29"/>
-      <c r="BJ7" s="29"/>
-      <c r="BK7" s="29"/>
-      <c r="BL7" s="29"/>
-      <c r="BM7" s="29"/>
-      <c r="BN7" s="29"/>
-      <c r="BO7" s="29"/>
-      <c r="BP7" s="29"/>
-    </row>
-    <row r="8" spans="1:68" ht="45" x14ac:dyDescent="0.2">
+      <c r="BG7" s="30"/>
+      <c r="BH7" s="30"/>
+      <c r="BI7" s="30"/>
+      <c r="BJ7" s="30"/>
+      <c r="BK7" s="30"/>
+      <c r="BL7" s="30"/>
+      <c r="BM7" s="30"/>
+      <c r="BN7" s="30"/>
+      <c r="BO7" s="30"/>
+      <c r="BP7" s="30"/>
+      <c r="BQ7" s="30"/>
+    </row>
+    <row r="8" spans="1:69" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>52</v>
       </c>
@@ -3070,199 +3247,202 @@
         <v>18</v>
       </c>
       <c r="E8" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="J8" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="K8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="6" t="s">
+      <c r="L8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="6" t="s">
+      <c r="M8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="N8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="O8" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="P8" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="Q8" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="R8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S8" s="10" t="s">
+      <c r="T8" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="U8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="U8" s="23" t="s">
+      <c r="V8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="V8" s="23" t="s">
+      <c r="W8" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="W8" s="23" t="s">
+      <c r="X8" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="X8" s="6" t="s">
+      <c r="Y8" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="Y8" s="6" t="s">
+      <c r="Z8" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="Z8" s="6" t="s">
+      <c r="AA8" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="AA8" s="23" t="s">
+      <c r="AB8" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="AB8" s="23" t="s">
+      <c r="AC8" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="AC8" s="23" t="s">
+      <c r="AD8" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="AD8" s="6" t="s">
+      <c r="AE8" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="AE8" s="6" t="s">
+      <c r="AF8" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="AF8" s="6" t="s">
+      <c r="AG8" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="AG8" s="23" t="s">
+      <c r="AH8" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="AH8" s="23" t="s">
+      <c r="AI8" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="AI8" s="23" t="s">
+      <c r="AJ8" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="AJ8" s="6" t="s">
+      <c r="AK8" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="AK8" s="6" t="s">
+      <c r="AL8" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="AL8" s="6" t="s">
+      <c r="AM8" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="AM8" s="23" t="s">
+      <c r="AN8" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="AN8" s="23" t="s">
+      <c r="AO8" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="AO8" s="23" t="s">
+      <c r="AP8" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="AP8" s="23" t="s">
+      <c r="AQ8" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="AQ8" s="23" t="s">
+      <c r="AR8" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="AR8" s="23" t="s">
+      <c r="AS8" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="AS8" s="6" t="s">
+      <c r="AT8" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="AT8" s="6" t="s">
+      <c r="AU8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="AU8" s="6" t="s">
+      <c r="AV8" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="AV8" s="23" t="s">
+      <c r="AW8" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="AW8" s="23" t="s">
+      <c r="AX8" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="AX8" s="23" t="s">
+      <c r="AY8" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="AY8" s="6" t="s">
+      <c r="AZ8" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="AZ8" s="6" t="s">
+      <c r="BA8" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="BA8" s="6" t="s">
+      <c r="BB8" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="BB8" s="23" t="s">
+      <c r="BC8" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="BC8" s="23" t="s">
+      <c r="BD8" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="BD8" s="23" t="s">
+      <c r="BE8" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="BE8" s="6" t="s">
+      <c r="BF8" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="BF8" s="6" t="s">
+      <c r="BG8" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="BG8" s="6" t="s">
+      <c r="BH8" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="BH8" s="23" t="s">
+      <c r="BI8" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="BI8" s="23" t="s">
+      <c r="BJ8" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="BJ8" s="23" t="s">
+      <c r="BK8" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="BK8" s="24" t="s">
+      <c r="BL8" s="24" t="s">
         <v>259</v>
       </c>
-      <c r="BL8" s="24" t="s">
+      <c r="BM8" s="24" t="s">
         <v>260</v>
       </c>
-      <c r="BM8" s="24" t="s">
+      <c r="BN8" s="24" t="s">
         <v>261</v>
       </c>
-      <c r="BN8" s="23" t="s">
+      <c r="BO8" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="BO8" s="23" t="s">
+      <c r="BP8" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="BP8" s="23" t="s">
+      <c r="BQ8" s="23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:68" ht="45" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:69" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>65</v>
       </c>
@@ -3273,138 +3453,145 @@
       <c r="D9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="7"/>
+      <c r="J9" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="K9" s="7"/>
       <c r="L9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="11"/>
+      <c r="M9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N9" s="7"/>
       <c r="O9" s="11"/>
       <c r="P9" s="11"/>
-      <c r="Q9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R9" s="7"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
-      <c r="U9" s="2" t="s">
+      <c r="U9" s="7"/>
+      <c r="V9" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="V9" s="2" t="s">
+      <c r="W9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2" t="s">
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="Y9" s="2" t="s">
+      <c r="Z9" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="Z9" s="2"/>
-      <c r="AA9" s="2" t="s">
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="AB9" s="2"/>
-      <c r="AC9" s="2"/>
-      <c r="AD9" s="2" t="s">
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AE9" s="2" t="s">
+      <c r="AF9" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AG9" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AG9" s="2" t="s">
+      <c r="AH9" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="AH9" s="2" t="s">
+      <c r="AI9" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="AI9" s="2"/>
-      <c r="AJ9" s="2" t="s">
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AK9" s="2" t="s">
+      <c r="AL9" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="AL9" s="2" t="s">
+      <c r="AM9" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AM9" s="2" t="s">
+      <c r="AN9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="AN9" s="2" t="s">
+      <c r="AO9" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="AO9" s="2"/>
-      <c r="AP9" s="2" t="s">
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AQ9" s="2" t="s">
+      <c r="AR9" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="2" t="s">
+      <c r="AS9" s="7"/>
+      <c r="AT9" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="AT9" s="2" t="s">
+      <c r="AU9" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="AU9" s="2"/>
-      <c r="AV9" s="2" t="s">
+      <c r="AV9" s="7"/>
+      <c r="AW9" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AW9" s="2"/>
-      <c r="AX9" s="2"/>
-      <c r="AY9" s="2" t="s">
+      <c r="AX9" s="7"/>
+      <c r="AY9" s="7"/>
+      <c r="AZ9" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="AZ9" s="2"/>
-      <c r="BA9" s="2"/>
-      <c r="BB9" s="2" t="s">
+      <c r="BA9" s="7"/>
+      <c r="BB9" s="7"/>
+      <c r="BC9" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="BC9" s="2" t="s">
+      <c r="BD9" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="BD9" s="2"/>
-      <c r="BE9" s="2" t="s">
+      <c r="BE9" s="7"/>
+      <c r="BF9" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="BF9" s="2" t="s">
+      <c r="BG9" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="BG9" s="2"/>
-      <c r="BH9" s="2" t="s">
+      <c r="BH9" s="7"/>
+      <c r="BI9" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="BI9" s="2" t="s">
+      <c r="BJ9" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="BJ9" s="2"/>
-      <c r="BK9" s="2"/>
-      <c r="BL9" s="2"/>
-      <c r="BM9" s="2"/>
-      <c r="BN9" s="2" t="s">
+      <c r="BK9" s="7"/>
+      <c r="BL9" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BM9" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="BN9" s="7"/>
+      <c r="BO9" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="BO9" s="2" t="s">
+      <c r="BP9" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="BP9" s="2"/>
-    </row>
-    <row r="10" spans="1:68" ht="45" x14ac:dyDescent="0.2">
+      <c r="BQ9" s="7"/>
+    </row>
+    <row r="10" spans="1:69" ht="45" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>65</v>
       </c>
@@ -3415,136 +3602,139 @@
       <c r="D10" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="K10" s="7"/>
       <c r="L10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="11"/>
+      <c r="M10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="7"/>
       <c r="O10" s="11"/>
       <c r="P10" s="11"/>
-      <c r="Q10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R10" s="7"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="2" t="s">
+      <c r="U10" s="7"/>
+      <c r="V10" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="V10" s="2" t="s">
+      <c r="W10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2" t="s">
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="Y10" s="2" t="s">
+      <c r="Z10" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2" t="s">
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="2"/>
-      <c r="AD10" s="2" t="s">
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AE10" s="2" t="s">
+      <c r="AF10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AG10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AG10" s="2" t="s">
+      <c r="AH10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AH10" s="2" t="s">
+      <c r="AI10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AI10" s="2"/>
-      <c r="AJ10" s="2" t="s">
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="AK10" s="2" t="s">
+      <c r="AL10" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="AL10" s="2"/>
-      <c r="AM10" s="2" t="s">
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="AN10" s="2" t="s">
+      <c r="AO10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AO10" s="2"/>
-      <c r="AP10" s="2" t="s">
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="AQ10" s="2" t="s">
+      <c r="AR10" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="2" t="s">
+      <c r="AS10" s="7"/>
+      <c r="AT10" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="AT10" s="2" t="s">
+      <c r="AU10" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="AU10" s="2" t="s">
+      <c r="AV10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AW10" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="AW10" s="2"/>
-      <c r="AX10" s="2"/>
-      <c r="AY10" s="2" t="s">
+      <c r="AX10" s="7"/>
+      <c r="AY10" s="7"/>
+      <c r="AZ10" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="AZ10" s="2"/>
-      <c r="BA10" s="2"/>
-      <c r="BB10" s="2"/>
-      <c r="BC10" s="2"/>
-      <c r="BD10" s="2"/>
-      <c r="BE10" s="2" t="s">
+      <c r="BA10" s="7"/>
+      <c r="BB10" s="7"/>
+      <c r="BC10" s="7"/>
+      <c r="BD10" s="7"/>
+      <c r="BE10" s="7"/>
+      <c r="BF10" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="BF10" s="2" t="s">
+      <c r="BG10" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="BG10" s="2" t="s">
+      <c r="BH10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="BH10" s="2" t="s">
+      <c r="BI10" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="BI10" s="2" t="s">
+      <c r="BJ10" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="BJ10" s="2"/>
-      <c r="BK10" s="2"/>
-      <c r="BL10" s="2"/>
-      <c r="BM10" s="2"/>
-      <c r="BN10" s="2" t="s">
+      <c r="BK10" s="7"/>
+      <c r="BL10" s="7"/>
+      <c r="BM10" s="7"/>
+      <c r="BN10" s="7"/>
+      <c r="BO10" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="BO10" s="2" t="s">
+      <c r="BP10" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="BP10" s="2"/>
-    </row>
-    <row r="11" spans="1:68" ht="45" x14ac:dyDescent="0.2">
+      <c r="BQ10" s="7"/>
+    </row>
+    <row r="11" spans="1:69" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>65</v>
       </c>
@@ -3555,106 +3745,109 @@
       <c r="D11" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="E11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="K11" s="7"/>
       <c r="L11" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M11" s="7"/>
-      <c r="N11" s="11"/>
+      <c r="M11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N11" s="7"/>
       <c r="O11" s="11"/>
       <c r="P11" s="11"/>
-      <c r="Q11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R11" s="7"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="2" t="s">
+      <c r="U11" s="7"/>
+      <c r="V11" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="V11" s="2" t="s">
+      <c r="W11" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2" t="s">
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="Y11" s="2" t="s">
+      <c r="Z11" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="Z11" s="2"/>
-      <c r="AA11" s="2" t="s">
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="AB11" s="2" t="s">
+      <c r="AC11" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="AC11" s="2"/>
-      <c r="AD11" s="2" t="s">
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AE11" s="2" t="s">
+      <c r="AF11" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AF11" s="2" t="s">
+      <c r="AG11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AG11" s="2" t="s">
+      <c r="AH11" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="AH11" s="2" t="s">
+      <c r="AI11" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="AI11" s="2"/>
-      <c r="AJ11" s="2" t="s">
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AK11" s="2" t="s">
+      <c r="AL11" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="AL11" s="2" t="s">
+      <c r="AM11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AM11" s="2"/>
-      <c r="AN11" s="2"/>
-      <c r="AO11" s="2"/>
-      <c r="AP11" s="2"/>
-      <c r="AQ11" s="2"/>
-      <c r="AR11" s="2"/>
-      <c r="AS11" s="2"/>
-      <c r="AT11" s="2"/>
-      <c r="AU11" s="2"/>
-      <c r="AV11" s="2"/>
-      <c r="AW11" s="2"/>
-      <c r="AX11" s="2"/>
-      <c r="AY11" s="2"/>
-      <c r="AZ11" s="2"/>
-      <c r="BA11" s="2"/>
-      <c r="BB11" s="2"/>
-      <c r="BC11" s="2"/>
-      <c r="BD11" s="2"/>
-      <c r="BE11" s="2"/>
-      <c r="BF11" s="2"/>
-      <c r="BG11" s="2"/>
-      <c r="BH11" s="2"/>
-      <c r="BI11" s="2"/>
-      <c r="BJ11" s="2"/>
-      <c r="BK11" s="2"/>
-      <c r="BL11" s="2"/>
-      <c r="BM11" s="2"/>
-      <c r="BN11" s="2"/>
-      <c r="BO11" s="2"/>
-      <c r="BP11" s="2"/>
-    </row>
-    <row r="12" spans="1:68" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="AN11" s="7"/>
+      <c r="AO11" s="7"/>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="7"/>
+      <c r="AR11" s="7"/>
+      <c r="AS11" s="7"/>
+      <c r="AT11" s="7"/>
+      <c r="AU11" s="7"/>
+      <c r="AV11" s="7"/>
+      <c r="AW11" s="7"/>
+      <c r="AX11" s="7"/>
+      <c r="AY11" s="7"/>
+      <c r="AZ11" s="7"/>
+      <c r="BA11" s="7"/>
+      <c r="BB11" s="7"/>
+      <c r="BC11" s="7"/>
+      <c r="BD11" s="7"/>
+      <c r="BE11" s="7"/>
+      <c r="BF11" s="7"/>
+      <c r="BG11" s="7"/>
+      <c r="BH11" s="7"/>
+      <c r="BI11" s="7"/>
+      <c r="BJ11" s="7"/>
+      <c r="BK11" s="7"/>
+      <c r="BL11" s="7"/>
+      <c r="BM11" s="7"/>
+      <c r="BN11" s="7"/>
+      <c r="BO11" s="7"/>
+      <c r="BP11" s="7"/>
+      <c r="BQ11" s="7"/>
+    </row>
+    <row r="12" spans="1:69" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>65</v>
       </c>
@@ -3665,108 +3858,111 @@
       <c r="D12" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="E12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="11"/>
+      <c r="N12" s="7"/>
       <c r="O12" s="11"/>
       <c r="P12" s="11"/>
-      <c r="Q12" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R12" s="7"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
-      <c r="U12" s="2" t="s">
+      <c r="U12" s="7"/>
+      <c r="V12" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="V12" s="2" t="s">
+      <c r="W12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="W12" s="2"/>
-      <c r="X12" s="2" t="s">
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="Z12" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="Z12" s="2"/>
-      <c r="AA12" s="2" t="s">
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="AB12" s="2" t="s">
+      <c r="AC12" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="2" t="s">
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AE12" s="2" t="s">
+      <c r="AF12" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AF12" s="2" t="s">
+      <c r="AG12" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AG12" s="2" t="s">
+      <c r="AH12" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="AH12" s="2" t="s">
+      <c r="AI12" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="AI12" s="2"/>
-      <c r="AJ12" s="2" t="s">
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="AK12" s="2" t="s">
+      <c r="AL12" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="AL12" s="2" t="s">
+      <c r="AM12" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AM12" s="2" t="s">
+      <c r="AN12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AN12" s="2" t="s">
+      <c r="AO12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AO12" s="2"/>
-      <c r="AP12" s="2"/>
-      <c r="AQ12" s="2"/>
-      <c r="AR12" s="2"/>
-      <c r="AS12" s="2"/>
-      <c r="AT12" s="2"/>
-      <c r="AU12" s="2"/>
-      <c r="AV12" s="2"/>
-      <c r="AW12" s="2"/>
-      <c r="AX12" s="2"/>
-      <c r="AY12" s="2"/>
-      <c r="AZ12" s="2"/>
-      <c r="BA12" s="2"/>
-      <c r="BB12" s="2"/>
-      <c r="BC12" s="2"/>
-      <c r="BD12" s="2"/>
-      <c r="BE12" s="2"/>
-      <c r="BF12" s="2"/>
-      <c r="BG12" s="2"/>
-      <c r="BH12" s="2"/>
-      <c r="BI12" s="2"/>
-      <c r="BJ12" s="2"/>
-      <c r="BK12" s="2"/>
-      <c r="BL12" s="2"/>
-      <c r="BM12" s="2"/>
-      <c r="BN12" s="2"/>
-      <c r="BO12" s="2"/>
-      <c r="BP12" s="2"/>
-    </row>
-    <row r="13" spans="1:68" ht="202.5" x14ac:dyDescent="0.2">
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="7"/>
+      <c r="AR12" s="7"/>
+      <c r="AS12" s="7"/>
+      <c r="AT12" s="7"/>
+      <c r="AU12" s="7"/>
+      <c r="AV12" s="7"/>
+      <c r="AW12" s="7"/>
+      <c r="AX12" s="7"/>
+      <c r="AY12" s="7"/>
+      <c r="AZ12" s="7"/>
+      <c r="BA12" s="7"/>
+      <c r="BB12" s="7"/>
+      <c r="BC12" s="7"/>
+      <c r="BD12" s="7"/>
+      <c r="BE12" s="7"/>
+      <c r="BF12" s="7"/>
+      <c r="BG12" s="7"/>
+      <c r="BH12" s="7"/>
+      <c r="BI12" s="7"/>
+      <c r="BJ12" s="7"/>
+      <c r="BK12" s="7"/>
+      <c r="BL12" s="7"/>
+      <c r="BM12" s="7"/>
+      <c r="BN12" s="7"/>
+      <c r="BO12" s="7"/>
+      <c r="BP12" s="7"/>
+      <c r="BQ12" s="7"/>
+    </row>
+    <row r="13" spans="1:69" ht="202.5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>65</v>
       </c>
@@ -3777,142 +3973,145 @@
       <c r="D13" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="7"/>
+      <c r="J13" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="7"/>
+      <c r="L13" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="M13" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M13" s="7"/>
-      <c r="N13" s="11"/>
+      <c r="N13" s="7"/>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
-      <c r="Q13" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R13" s="7"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
-      <c r="U13" s="2" t="s">
+      <c r="U13" s="7"/>
+      <c r="V13" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="V13" s="2" t="s">
+      <c r="W13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="W13" s="2"/>
-      <c r="X13" s="2" t="s">
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Z13" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="Z13" s="2"/>
-      <c r="AA13" s="2" t="s">
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2" t="s">
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AE13" s="2" t="s">
+      <c r="AF13" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AF13" s="2" t="s">
+      <c r="AG13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AG13" s="2" t="s">
+      <c r="AH13" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="AH13" s="2" t="s">
+      <c r="AI13" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="AI13" s="2" t="s">
+      <c r="AJ13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AJ13" s="2" t="s">
+      <c r="AK13" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="AK13" s="2" t="s">
+      <c r="AL13" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="AL13" s="2" t="s">
+      <c r="AM13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AM13" s="2" t="s">
+      <c r="AN13" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="AN13" s="2" t="s">
+      <c r="AO13" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="AO13" s="2"/>
-      <c r="AP13" s="2" t="s">
+      <c r="AP13" s="7"/>
+      <c r="AQ13" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="AQ13" s="2" t="s">
+      <c r="AR13" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="AR13" s="2"/>
-      <c r="AS13" s="2" t="s">
+      <c r="AS13" s="7"/>
+      <c r="AT13" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="AT13" s="2" t="s">
+      <c r="AU13" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="AU13" s="2" t="s">
+      <c r="AV13" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AV13" s="2" t="s">
+      <c r="AW13" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="AW13" s="2"/>
-      <c r="AX13" s="2"/>
-      <c r="AY13" s="2" t="s">
+      <c r="AX13" s="7"/>
+      <c r="AY13" s="7"/>
+      <c r="AZ13" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="AZ13" s="2"/>
-      <c r="BA13" s="2"/>
-      <c r="BB13" s="2" t="s">
+      <c r="BA13" s="7"/>
+      <c r="BB13" s="7"/>
+      <c r="BC13" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="BC13" s="2" t="s">
+      <c r="BD13" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="BD13" s="2"/>
-      <c r="BE13" s="2" t="s">
+      <c r="BE13" s="7"/>
+      <c r="BF13" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="BF13" s="2" t="s">
+      <c r="BG13" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="BG13" s="2"/>
-      <c r="BH13" s="2" t="s">
+      <c r="BH13" s="7"/>
+      <c r="BI13" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="BI13" s="2" t="s">
+      <c r="BJ13" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="BJ13" s="2"/>
-      <c r="BK13" s="2"/>
-      <c r="BL13" s="2"/>
-      <c r="BM13" s="2"/>
-      <c r="BN13" s="2" t="s">
+      <c r="BK13" s="7"/>
+      <c r="BL13" s="7"/>
+      <c r="BM13" s="7"/>
+      <c r="BN13" s="7"/>
+      <c r="BO13" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="BO13" s="2" t="s">
+      <c r="BP13" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="BP13" s="2"/>
-    </row>
-    <row r="14" spans="1:68" ht="146.25" x14ac:dyDescent="0.2">
+      <c r="BQ13" s="7"/>
+    </row>
+    <row r="14" spans="1:69" ht="146.25" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>65</v>
       </c>
@@ -3923,108 +4122,111 @@
       <c r="D14" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="7"/>
+      <c r="L14" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="M14" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M14" s="7"/>
-      <c r="N14" s="11"/>
+      <c r="N14" s="7"/>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
-      <c r="Q14" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R14" s="7"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
-      <c r="U14" s="2" t="s">
+      <c r="U14" s="7"/>
+      <c r="V14" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="V14" s="2" t="s">
+      <c r="W14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="W14" s="2"/>
-      <c r="X14" s="2" t="s">
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="Y14" s="2" t="s">
+      <c r="Z14" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="Z14" s="2"/>
-      <c r="AA14" s="2" t="s">
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="AB14" s="2" t="s">
+      <c r="AC14" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2" t="s">
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="AE14" s="2" t="s">
+      <c r="AF14" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="AF14" s="2" t="s">
+      <c r="AG14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AG14" s="2">
+      <c r="AH14" s="7">
         <v>0.6</v>
       </c>
-      <c r="AH14" s="2">
+      <c r="AI14" s="7">
         <v>0</v>
       </c>
-      <c r="AI14" s="2"/>
-      <c r="AJ14" s="2" t="s">
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="AK14" s="2" t="s">
+      <c r="AL14" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="AL14" s="2"/>
-      <c r="AM14" s="2">
+      <c r="AM14" s="7"/>
+      <c r="AN14" s="7">
         <v>0</v>
       </c>
-      <c r="AN14" s="2">
+      <c r="AO14" s="7">
         <v>0</v>
       </c>
-      <c r="AO14" s="2"/>
-      <c r="AP14" s="2"/>
-      <c r="AQ14" s="2"/>
-      <c r="AR14" s="2"/>
-      <c r="AS14" s="2"/>
-      <c r="AT14" s="2"/>
-      <c r="AU14" s="2"/>
-      <c r="AV14" s="2"/>
-      <c r="AW14" s="2"/>
-      <c r="AX14" s="2"/>
-      <c r="AY14" s="2"/>
-      <c r="AZ14" s="2"/>
-      <c r="BA14" s="2"/>
-      <c r="BB14" s="2"/>
-      <c r="BC14" s="2"/>
-      <c r="BD14" s="2"/>
-      <c r="BE14" s="2"/>
-      <c r="BF14" s="2"/>
-      <c r="BG14" s="2"/>
-      <c r="BH14" s="2"/>
-      <c r="BI14" s="2"/>
-      <c r="BJ14" s="2"/>
-      <c r="BK14" s="2"/>
-      <c r="BL14" s="2"/>
-      <c r="BM14" s="2"/>
-      <c r="BN14" s="2"/>
-      <c r="BO14" s="2"/>
-      <c r="BP14" s="2"/>
-    </row>
-    <row r="15" spans="1:68" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7"/>
+      <c r="AR14" s="7"/>
+      <c r="AS14" s="7"/>
+      <c r="AT14" s="7"/>
+      <c r="AU14" s="7"/>
+      <c r="AV14" s="7"/>
+      <c r="AW14" s="7"/>
+      <c r="AX14" s="7"/>
+      <c r="AY14" s="7"/>
+      <c r="AZ14" s="7"/>
+      <c r="BA14" s="7"/>
+      <c r="BB14" s="7"/>
+      <c r="BC14" s="7"/>
+      <c r="BD14" s="7"/>
+      <c r="BE14" s="7"/>
+      <c r="BF14" s="7"/>
+      <c r="BG14" s="7"/>
+      <c r="BH14" s="7"/>
+      <c r="BI14" s="7"/>
+      <c r="BJ14" s="7"/>
+      <c r="BK14" s="7"/>
+      <c r="BL14" s="7"/>
+      <c r="BM14" s="7"/>
+      <c r="BN14" s="7"/>
+      <c r="BO14" s="7"/>
+      <c r="BP14" s="7"/>
+      <c r="BQ14" s="7"/>
+    </row>
+    <row r="15" spans="1:69" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>65</v>
       </c>
@@ -4035,140 +4237,147 @@
       <c r="D15" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="7"/>
+      <c r="J15" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="K15" s="7"/>
       <c r="L15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M15" s="7"/>
-      <c r="N15" s="11"/>
+      <c r="M15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N15" s="7"/>
       <c r="O15" s="11"/>
       <c r="P15" s="11"/>
-      <c r="Q15" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R15" s="7"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
-      <c r="U15" s="2">
+      <c r="U15" s="7"/>
+      <c r="V15" s="7">
         <v>0.04</v>
       </c>
-      <c r="V15" s="2">
+      <c r="W15" s="7">
         <v>0</v>
       </c>
-      <c r="W15" s="2"/>
-      <c r="X15" s="2">
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7">
         <v>1</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Z15" s="7">
         <v>0.1</v>
       </c>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2" t="s">
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2" t="s">
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AE15" s="2" t="s">
+      <c r="AF15" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AF15" s="2" t="s">
+      <c r="AG15" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AG15" s="2" t="s">
+      <c r="AH15" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="AH15" s="2" t="s">
+      <c r="AI15" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="AI15" s="2"/>
-      <c r="AJ15" s="2" t="s">
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AK15" s="2" t="s">
+      <c r="AL15" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="AL15" s="2" t="s">
+      <c r="AM15" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AM15" s="2">
+      <c r="AN15" s="7">
         <v>1</v>
       </c>
-      <c r="AN15" s="2">
+      <c r="AO15" s="7">
         <v>0</v>
       </c>
-      <c r="AO15" s="2"/>
-      <c r="AP15" s="2">
+      <c r="AP15" s="7"/>
+      <c r="AQ15" s="7">
         <v>0</v>
       </c>
-      <c r="AQ15" s="2">
+      <c r="AR15" s="7">
         <v>0.75</v>
       </c>
-      <c r="AR15" s="2"/>
-      <c r="AS15" s="2">
+      <c r="AS15" s="7"/>
+      <c r="AT15" s="7">
         <v>180</v>
       </c>
-      <c r="AT15" s="2">
+      <c r="AU15" s="7">
         <v>90</v>
       </c>
-      <c r="AU15" s="2"/>
-      <c r="AV15" s="2">
+      <c r="AV15" s="7"/>
+      <c r="AW15" s="7">
         <v>1000</v>
       </c>
-      <c r="AW15" s="2"/>
-      <c r="AX15" s="2"/>
-      <c r="AY15" s="2">
+      <c r="AX15" s="7"/>
+      <c r="AY15" s="7"/>
+      <c r="AZ15" s="7">
         <v>0</v>
       </c>
-      <c r="AZ15" s="2">
+      <c r="BA15" s="7">
         <v>0</v>
       </c>
-      <c r="BA15" s="2"/>
-      <c r="BB15" s="2">
+      <c r="BB15" s="7"/>
+      <c r="BC15" s="7">
         <v>0</v>
       </c>
-      <c r="BC15" s="2">
+      <c r="BD15" s="7">
         <v>0</v>
       </c>
-      <c r="BD15" s="2"/>
-      <c r="BE15" s="2">
+      <c r="BE15" s="7"/>
+      <c r="BF15" s="7">
         <v>20</v>
       </c>
-      <c r="BF15" s="2">
+      <c r="BG15" s="7">
         <v>8</v>
       </c>
-      <c r="BG15" s="2"/>
-      <c r="BH15" s="2">
+      <c r="BH15" s="7"/>
+      <c r="BI15" s="7">
         <v>0.35</v>
       </c>
-      <c r="BI15" s="2">
+      <c r="BJ15" s="7">
         <v>0.35</v>
       </c>
-      <c r="BJ15" s="2"/>
-      <c r="BK15" s="2"/>
-      <c r="BL15" s="2"/>
-      <c r="BM15" s="2"/>
-      <c r="BN15" s="2" t="s">
+      <c r="BK15" s="7"/>
+      <c r="BL15" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="BM15" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="BN15" s="7"/>
+      <c r="BO15" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="BO15" s="2" t="s">
+      <c r="BP15" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="BP15" s="2"/>
-    </row>
-    <row r="16" spans="1:68" ht="45" x14ac:dyDescent="0.2">
+      <c r="BQ15" s="7"/>
+    </row>
+    <row r="16" spans="1:69" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>65</v>
       </c>
@@ -4179,146 +4388,149 @@
       <c r="D16" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="7"/>
+      <c r="J16" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="K16" s="7"/>
       <c r="L16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="M16" s="7"/>
-      <c r="N16" s="11"/>
+      <c r="M16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="N16" s="7"/>
       <c r="O16" s="11"/>
       <c r="P16" s="11"/>
-      <c r="Q16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="R16" s="7"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="7" t="s">
+        <v>272</v>
+      </c>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
-      <c r="U16" s="2">
+      <c r="U16" s="7"/>
+      <c r="V16" s="7">
         <v>0.04</v>
       </c>
-      <c r="V16" s="2">
+      <c r="W16" s="7">
         <v>0</v>
       </c>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2">
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7">
         <v>1</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Z16" s="7">
         <v>0.1</v>
       </c>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2" t="s">
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="2"/>
-      <c r="AD16" s="2" t="s">
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AF16" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="AF16" s="2" t="s">
+      <c r="AG16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AG16" s="2" t="s">
+      <c r="AH16" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="AH16" s="2" t="s">
+      <c r="AI16" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="AI16" s="2"/>
-      <c r="AJ16" s="2" t="s">
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="AK16" s="2" t="s">
+      <c r="AL16" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="AL16" s="2" t="s">
+      <c r="AM16" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="AM16" s="2">
+      <c r="AN16" s="7">
         <v>1</v>
       </c>
-      <c r="AN16" s="2">
+      <c r="AO16" s="7">
         <v>0</v>
       </c>
-      <c r="AO16" s="2"/>
-      <c r="AP16" s="2">
+      <c r="AP16" s="7"/>
+      <c r="AQ16" s="7">
         <v>0.75</v>
       </c>
-      <c r="AQ16" s="2">
+      <c r="AR16" s="7">
         <v>0.7</v>
       </c>
-      <c r="AR16" s="2" t="s">
+      <c r="AS16" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="AS16" s="2">
+      <c r="AT16" s="7">
         <v>40</v>
       </c>
-      <c r="AT16" s="2">
+      <c r="AU16" s="7">
         <v>10</v>
       </c>
-      <c r="AU16" s="2"/>
-      <c r="AV16" s="2">
+      <c r="AV16" s="7"/>
+      <c r="AW16" s="7">
         <v>1000</v>
       </c>
-      <c r="AW16" s="2"/>
-      <c r="AX16" s="2"/>
-      <c r="AY16" s="2">
+      <c r="AX16" s="7"/>
+      <c r="AY16" s="7"/>
+      <c r="AZ16" s="7">
         <v>0</v>
       </c>
-      <c r="AZ16" s="2">
+      <c r="BA16" s="7">
         <v>0</v>
       </c>
-      <c r="BA16" s="2"/>
-      <c r="BB16" s="2">
+      <c r="BB16" s="7"/>
+      <c r="BC16" s="7">
         <v>0</v>
       </c>
-      <c r="BC16" s="2">
+      <c r="BD16" s="7">
         <v>0</v>
       </c>
-      <c r="BD16" s="2"/>
-      <c r="BE16" s="2">
+      <c r="BE16" s="7"/>
+      <c r="BF16" s="7">
         <v>8</v>
       </c>
-      <c r="BF16" s="2">
+      <c r="BG16" s="7">
         <v>3</v>
       </c>
-      <c r="BG16" s="2"/>
-      <c r="BH16" s="2">
+      <c r="BH16" s="7"/>
+      <c r="BI16" s="7">
         <v>0</v>
       </c>
-      <c r="BI16" s="2">
+      <c r="BJ16" s="7">
         <v>0.25</v>
       </c>
-      <c r="BJ16" s="2"/>
-      <c r="BK16" s="2">
+      <c r="BK16" s="7"/>
+      <c r="BL16" s="7">
         <v>0</v>
       </c>
-      <c r="BL16" s="2">
+      <c r="BM16" s="7">
         <v>0.25</v>
       </c>
-      <c r="BM16" s="2"/>
-      <c r="BN16" s="2" t="s">
+      <c r="BN16" s="7"/>
+      <c r="BO16" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="BO16" s="2" t="s">
+      <c r="BP16" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="BP16" s="2"/>
-    </row>
-    <row r="17" spans="1:68" ht="15" x14ac:dyDescent="0.2">
+      <c r="BQ16" s="7"/>
+    </row>
+    <row r="17" spans="1:69" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="20"/>
@@ -4332,149 +4544,163 @@
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
-      <c r="N17" s="11"/>
+      <c r="N17" s="7"/>
       <c r="O17" s="11"/>
       <c r="P17" s="11"/>
-      <c r="Q17" s="7"/>
+      <c r="Q17" s="11"/>
       <c r="R17" s="7"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
-      <c r="Z17" s="2"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="2"/>
-      <c r="AD17" s="2"/>
-      <c r="AE17" s="2"/>
-      <c r="AF17" s="2"/>
-      <c r="AG17" s="2"/>
-      <c r="AH17" s="2"/>
-      <c r="AI17" s="2"/>
-      <c r="AJ17" s="2"/>
-      <c r="AK17" s="2"/>
-      <c r="AL17" s="2"/>
-      <c r="AM17" s="2"/>
-      <c r="AN17" s="2"/>
-      <c r="AO17" s="2"/>
-      <c r="AP17" s="2"/>
-      <c r="AQ17" s="2"/>
-      <c r="AR17" s="2"/>
-      <c r="AS17" s="2"/>
-      <c r="AT17" s="2"/>
-      <c r="AU17" s="2"/>
-      <c r="AV17" s="2"/>
-      <c r="AW17" s="2"/>
-      <c r="AX17" s="2"/>
-      <c r="AY17" s="2"/>
-      <c r="AZ17" s="2"/>
-      <c r="BA17" s="2"/>
-      <c r="BB17" s="2"/>
-      <c r="BC17" s="2"/>
-      <c r="BD17" s="2"/>
-      <c r="BE17" s="2"/>
-      <c r="BF17" s="2"/>
-      <c r="BG17" s="2"/>
-      <c r="BH17" s="2"/>
-      <c r="BI17" s="2"/>
-      <c r="BJ17" s="2"/>
-      <c r="BK17" s="2"/>
-      <c r="BL17" s="2"/>
-      <c r="BM17" s="2"/>
-      <c r="BN17" s="2"/>
-      <c r="BO17" s="2"/>
-      <c r="BP17" s="2"/>
-    </row>
-    <row r="18" spans="1:68" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7"/>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="7"/>
+      <c r="AK17" s="7"/>
+      <c r="AL17" s="7"/>
+      <c r="AM17" s="7"/>
+      <c r="AN17" s="7"/>
+      <c r="AO17" s="7"/>
+      <c r="AP17" s="7"/>
+      <c r="AQ17" s="7"/>
+      <c r="AR17" s="7"/>
+      <c r="AS17" s="7"/>
+      <c r="AT17" s="7"/>
+      <c r="AU17" s="7"/>
+      <c r="AV17" s="7"/>
+      <c r="AW17" s="7"/>
+      <c r="AX17" s="7"/>
+      <c r="AY17" s="7"/>
+      <c r="AZ17" s="7"/>
+      <c r="BA17" s="7"/>
+      <c r="BB17" s="7"/>
+      <c r="BC17" s="7"/>
+      <c r="BD17" s="7"/>
+      <c r="BE17" s="7"/>
+      <c r="BF17" s="7"/>
+      <c r="BG17" s="7"/>
+      <c r="BH17" s="7"/>
+      <c r="BI17" s="7"/>
+      <c r="BJ17" s="7"/>
+      <c r="BK17" s="7"/>
+      <c r="BL17" s="7"/>
+      <c r="BM17" s="7"/>
+      <c r="BN17" s="7"/>
+      <c r="BO17" s="7"/>
+      <c r="BP17" s="7"/>
+      <c r="BQ17" s="7"/>
+    </row>
+    <row r="18" spans="1:69" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="B18" s="7"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>276</v>
+      </c>
       <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="K18" s="7" t="s">
+        <v>271</v>
+      </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="11"/>
+      <c r="N18" s="7"/>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
-      <c r="Q18" s="7"/>
+      <c r="Q18" s="11"/>
       <c r="R18" s="7"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
-      <c r="AL18" s="2"/>
-      <c r="AM18" s="2"/>
-      <c r="AN18" s="2"/>
-      <c r="AO18" s="2"/>
-      <c r="AP18" s="2"/>
-      <c r="AQ18" s="2"/>
-      <c r="AR18" s="2"/>
-      <c r="AS18" s="2"/>
-      <c r="AT18" s="2"/>
-      <c r="AU18" s="2"/>
-      <c r="AV18" s="2"/>
-      <c r="AW18" s="2"/>
-      <c r="AX18" s="2"/>
-      <c r="AY18" s="2"/>
-      <c r="AZ18" s="2"/>
-      <c r="BA18" s="2"/>
-      <c r="BB18" s="2"/>
-      <c r="BC18" s="2"/>
-      <c r="BD18" s="2"/>
-      <c r="BE18" s="2"/>
-      <c r="BF18" s="2"/>
-      <c r="BG18" s="2"/>
-      <c r="BH18" s="2"/>
-      <c r="BI18" s="2"/>
-      <c r="BJ18" s="2"/>
-      <c r="BK18" s="2"/>
-      <c r="BL18" s="2"/>
-      <c r="BM18" s="2"/>
-      <c r="BN18" s="2"/>
-      <c r="BO18" s="2"/>
-      <c r="BP18" s="2"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="7"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="7"/>
+      <c r="AJ18" s="7"/>
+      <c r="AK18" s="7"/>
+      <c r="AL18" s="7"/>
+      <c r="AM18" s="7"/>
+      <c r="AN18" s="7"/>
+      <c r="AO18" s="7"/>
+      <c r="AP18" s="7"/>
+      <c r="AQ18" s="7"/>
+      <c r="AR18" s="7"/>
+      <c r="AS18" s="7"/>
+      <c r="AT18" s="7"/>
+      <c r="AU18" s="7"/>
+      <c r="AV18" s="7"/>
+      <c r="AW18" s="7"/>
+      <c r="AX18" s="7"/>
+      <c r="AY18" s="7"/>
+      <c r="AZ18" s="7"/>
+      <c r="BA18" s="7"/>
+      <c r="BB18" s="7"/>
+      <c r="BC18" s="7"/>
+      <c r="BD18" s="7"/>
+      <c r="BE18" s="7"/>
+      <c r="BF18" s="7"/>
+      <c r="BG18" s="7"/>
+      <c r="BH18" s="7"/>
+      <c r="BI18" s="7"/>
+      <c r="BJ18" s="7"/>
+      <c r="BK18" s="7"/>
+      <c r="BL18" s="7"/>
+      <c r="BM18" s="7"/>
+      <c r="BN18" s="7"/>
+      <c r="BO18" s="7"/>
+      <c r="BP18" s="7"/>
+      <c r="BQ18" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="AG7:AR7"/>
-    <mergeCell ref="AS7:BD7"/>
-    <mergeCell ref="BE7:BP7"/>
+    <mergeCell ref="AH7:AS7"/>
+    <mergeCell ref="AT7:BE7"/>
+    <mergeCell ref="BF7:BQ7"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="K7:P7"/>
-    <mergeCell ref="Q7:S7"/>
-    <mergeCell ref="U7:AF7"/>
+    <mergeCell ref="L7:Q7"/>
+    <mergeCell ref="R7:T7"/>
+    <mergeCell ref="V7:AG7"/>
   </mergeCells>
-  <conditionalFormatting sqref="A9:BP18">
-    <cfRule type="notContainsBlanks" dxfId="27" priority="3">
+  <conditionalFormatting sqref="A9:BQ18">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A9))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B18">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="OFF">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="OFF">
       <formula>NOT(ISERROR(SEARCH("OFF",B9)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>